<commit_message>
First Push as of Feb 25, 2025 at 1:38 PM
</commit_message>
<xml_diff>
--- a/res/excel/set_per_item_bases/set_per_item.xlsx
+++ b/res/excel/set_per_item_bases/set_per_item.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldri\OneDrive\Desktop\WLP_Automation-v5\res\excel\set_per_item_bases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldri\OneDrive\Desktop\Nikka System\WLP_Automation-v7\res\excel\set_per_item_bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE509721-F5B0-49FB-B64C-73AD89BC736C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF80C5E-8CDF-4C1A-AC9F-6CD3902C8F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D8BCDB13-438F-4401-9ED9-1D96E22860A8}"/>
   </bookViews>
@@ -814,48 +814,6 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -863,6 +821,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -872,27 +872,7 @@
     <cellStyle name="Normal 3" xfId="2" xr:uid="{AAC69D67-66EA-4505-BD7B-4F7380F3F09B}"/>
     <cellStyle name="Normal 4" xfId="1" xr:uid="{8700A739-0731-49FA-BB7B-D8DB27A1C370}"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1226,8 +1206,8 @@
   <dimension ref="A1:EQ7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EA10" sqref="EA10"/>
+      <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CI2" sqref="CI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,170 +1221,170 @@
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="28" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="29" t="s">
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="AO1" s="29"/>
-      <c r="AP1" s="29"/>
-      <c r="AQ1" s="29"/>
-      <c r="AR1" s="29"/>
-      <c r="AS1" s="29"/>
-      <c r="AT1" s="29"/>
-      <c r="AU1" s="29"/>
-      <c r="AV1" s="29"/>
-      <c r="AW1" s="29"/>
-      <c r="AX1" s="29"/>
-      <c r="AY1" s="29"/>
-      <c r="AZ1" s="29"/>
-      <c r="BA1" s="29"/>
-      <c r="BB1" s="29"/>
-      <c r="BC1" s="29"/>
-      <c r="BD1" s="29"/>
-      <c r="BE1" s="29"/>
-      <c r="BF1" s="29"/>
-      <c r="BG1" s="30" t="s">
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
-      <c r="BQ1" s="31"/>
-      <c r="BR1" s="31"/>
-      <c r="BS1" s="31"/>
-      <c r="BT1" s="32"/>
-      <c r="BU1" s="33" t="s">
+      <c r="BH1" s="34"/>
+      <c r="BI1" s="34"/>
+      <c r="BJ1" s="34"/>
+      <c r="BK1" s="34"/>
+      <c r="BL1" s="34"/>
+      <c r="BM1" s="34"/>
+      <c r="BN1" s="34"/>
+      <c r="BO1" s="34"/>
+      <c r="BP1" s="34"/>
+      <c r="BQ1" s="34"/>
+      <c r="BR1" s="34"/>
+      <c r="BS1" s="34"/>
+      <c r="BT1" s="35"/>
+      <c r="BU1" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="BV1" s="34"/>
-      <c r="BW1" s="34"/>
-      <c r="BX1" s="34"/>
-      <c r="BY1" s="34"/>
-      <c r="BZ1" s="34"/>
-      <c r="CA1" s="34"/>
-      <c r="CB1" s="34"/>
-      <c r="CC1" s="34"/>
-      <c r="CD1" s="34"/>
-      <c r="CE1" s="35"/>
-      <c r="CF1" s="23" t="s">
+      <c r="BV1" s="37"/>
+      <c r="BW1" s="37"/>
+      <c r="BX1" s="37"/>
+      <c r="BY1" s="37"/>
+      <c r="BZ1" s="37"/>
+      <c r="CA1" s="37"/>
+      <c r="CB1" s="37"/>
+      <c r="CC1" s="37"/>
+      <c r="CD1" s="37"/>
+      <c r="CE1" s="38"/>
+      <c r="CF1" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="CG1" s="23"/>
-      <c r="CH1" s="23"/>
-      <c r="CI1" s="23"/>
-      <c r="CJ1" s="23"/>
-      <c r="CK1" s="23"/>
-      <c r="CL1" s="23"/>
-      <c r="CM1" s="23"/>
-      <c r="CN1" s="23"/>
-      <c r="CO1" s="23"/>
-      <c r="CP1" s="24" t="s">
+      <c r="CG1" s="26"/>
+      <c r="CH1" s="26"/>
+      <c r="CI1" s="26"/>
+      <c r="CJ1" s="26"/>
+      <c r="CK1" s="26"/>
+      <c r="CL1" s="26"/>
+      <c r="CM1" s="26"/>
+      <c r="CN1" s="26"/>
+      <c r="CO1" s="26"/>
+      <c r="CP1" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="CQ1" s="25"/>
-      <c r="CR1" s="25"/>
-      <c r="CS1" s="25"/>
-      <c r="CT1" s="25"/>
-      <c r="CU1" s="26"/>
-      <c r="CV1" s="22" t="s">
+      <c r="CQ1" s="28"/>
+      <c r="CR1" s="28"/>
+      <c r="CS1" s="28"/>
+      <c r="CT1" s="28"/>
+      <c r="CU1" s="29"/>
+      <c r="CV1" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="CW1" s="22"/>
-      <c r="CX1" s="22"/>
-      <c r="CY1" s="22"/>
-      <c r="CZ1" s="22"/>
-      <c r="DA1" s="22"/>
-      <c r="DB1" s="22"/>
-      <c r="DC1" s="22"/>
-      <c r="DD1" s="22"/>
-      <c r="DE1" s="22"/>
-      <c r="DF1" s="22"/>
-      <c r="DG1" s="22"/>
-      <c r="DH1" s="22"/>
-      <c r="DI1" s="22"/>
-      <c r="DJ1" s="22"/>
-      <c r="DK1" s="22"/>
-      <c r="DL1" s="22"/>
-      <c r="DM1" s="22"/>
-      <c r="DN1" s="22"/>
-      <c r="DO1" s="37" t="s">
+      <c r="CW1" s="25"/>
+      <c r="CX1" s="25"/>
+      <c r="CY1" s="25"/>
+      <c r="CZ1" s="25"/>
+      <c r="DA1" s="25"/>
+      <c r="DB1" s="25"/>
+      <c r="DC1" s="25"/>
+      <c r="DD1" s="25"/>
+      <c r="DE1" s="25"/>
+      <c r="DF1" s="25"/>
+      <c r="DG1" s="25"/>
+      <c r="DH1" s="25"/>
+      <c r="DI1" s="25"/>
+      <c r="DJ1" s="25"/>
+      <c r="DK1" s="25"/>
+      <c r="DL1" s="25"/>
+      <c r="DM1" s="25"/>
+      <c r="DN1" s="25"/>
+      <c r="DO1" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="DP1" s="38"/>
-      <c r="DQ1" s="38"/>
-      <c r="DR1" s="38"/>
-      <c r="DS1" s="38"/>
-      <c r="DT1" s="38"/>
-      <c r="DU1" s="38"/>
-      <c r="DV1" s="38"/>
-      <c r="DW1" s="38"/>
-      <c r="DX1" s="38"/>
-      <c r="DY1" s="38"/>
-      <c r="DZ1" s="38"/>
-      <c r="EA1" s="38"/>
-      <c r="EB1" s="38"/>
-      <c r="EC1" s="38"/>
-      <c r="ED1" s="38"/>
-      <c r="EE1" s="38"/>
-      <c r="EF1" s="38"/>
-      <c r="EG1" s="38"/>
-      <c r="EH1" s="38"/>
-      <c r="EI1" s="38"/>
-      <c r="EJ1" s="38"/>
-      <c r="EK1" s="38"/>
-      <c r="EL1" s="38"/>
-      <c r="EM1" s="38"/>
-      <c r="EN1" s="38"/>
-      <c r="EO1" s="38"/>
-      <c r="EP1" s="38"/>
-      <c r="EQ1" s="38"/>
+      <c r="DP1" s="24"/>
+      <c r="DQ1" s="24"/>
+      <c r="DR1" s="24"/>
+      <c r="DS1" s="24"/>
+      <c r="DT1" s="24"/>
+      <c r="DU1" s="24"/>
+      <c r="DV1" s="24"/>
+      <c r="DW1" s="24"/>
+      <c r="DX1" s="24"/>
+      <c r="DY1" s="24"/>
+      <c r="DZ1" s="24"/>
+      <c r="EA1" s="24"/>
+      <c r="EB1" s="24"/>
+      <c r="EC1" s="24"/>
+      <c r="ED1" s="24"/>
+      <c r="EE1" s="24"/>
+      <c r="EF1" s="24"/>
+      <c r="EG1" s="24"/>
+      <c r="EH1" s="24"/>
+      <c r="EI1" s="24"/>
+      <c r="EJ1" s="24"/>
+      <c r="EK1" s="24"/>
+      <c r="EL1" s="24"/>
+      <c r="EM1" s="24"/>
+      <c r="EN1" s="24"/>
+      <c r="EO1" s="24"/>
+      <c r="EP1" s="24"/>
+      <c r="EQ1" s="24"/>
     </row>
     <row r="2" spans="1:147" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1845,7 +1825,7 @@
       <c r="EP2" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="EQ2" s="36" t="s">
+      <c r="EQ2" s="22" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3152,6 +3132,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="DO1:EQ1"/>
     <mergeCell ref="CV1:DN1"/>
     <mergeCell ref="CF1:CO1"/>
     <mergeCell ref="CP1:CU1"/>
@@ -3160,10 +3141,9 @@
     <mergeCell ref="AN1:BF1"/>
     <mergeCell ref="BG1:BT1"/>
     <mergeCell ref="BU1:CE1"/>
-    <mergeCell ref="DO1:EQ1"/>
   </mergeCells>
   <conditionalFormatting sqref="DO2:EQ2">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3265,7 +3245,7 @@
       <c r="AB1" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="AC1" s="36" t="s">
+      <c r="AC1" s="22" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3544,7 +3524,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>